<commit_message>
optimized code and applied ngxSpinnerservies
</commit_message>
<xml_diff>
--- a/Documentation/Database snapshot.xlsx
+++ b/Documentation/Database snapshot.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MET\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F23A17BE-F1FD-4E2D-A085-85BC4A147E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630AB1D7-CC1E-4D6D-AA5E-3E6D8B333008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E627DE3D-8FED-48C3-8A35-A50FBDD7FFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Modules" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>shobhit</t>
   </si>
@@ -82,6 +82,66 @@
   </si>
   <si>
     <t>it</t>
+  </si>
+  <si>
+    <t>Training of Trainer &amp; Training of Assessor</t>
+  </si>
+  <si>
+    <t>Qualification Pack – National Occupational Standard Builder</t>
+  </si>
+  <si>
+    <t>Center Accreditation and Affiliation Module</t>
+  </si>
+  <si>
+    <t>Candidate Self Registration and Candidate Login and Profile Management</t>
+  </si>
+  <si>
+    <t>Fee Based Module</t>
+  </si>
+  <si>
+    <t>NON PMKVY Module</t>
+  </si>
+  <si>
+    <t>Rozgar Mela</t>
+  </si>
+  <si>
+    <t>TP – TC Onboarding and Target Allocation</t>
+  </si>
+  <si>
+    <t>Candidate Training Lifecycle</t>
+  </si>
+  <si>
+    <t>Batch Creation and Candidate Enrollment</t>
+  </si>
+  <si>
+    <t>Assessment, Re-Assessment and Certification</t>
+  </si>
+  <si>
+    <t>Budget and Payout</t>
+  </si>
+  <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Continuous Monitoring</t>
+  </si>
+  <si>
+    <t>Third Party Integrations</t>
+  </si>
+  <si>
+    <t>API Integration - States</t>
+  </si>
+  <si>
+    <t>API Integration - Central Ministry</t>
+  </si>
+  <si>
+    <t>Nano BI Report</t>
+  </si>
+  <si>
+    <t>Nano BI Dashboard</t>
+  </si>
+  <si>
+    <t>Excel Report</t>
   </si>
 </sst>
 </file>
@@ -581,12 +641,299 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF863948-2424-4208-B311-6F0B1FAC2191}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44043.942811365741</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44043.943102164354</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44043.943250995369</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44043.944480011574</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44043.944788506946</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44043.94494342593</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44043.945096261574</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44043.945341944447</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44043.945489398146</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44043.945682604164</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44043.945906215275</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44043.946069409722</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44043.946205601853</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44043.946392812497</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44043.946536469906</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44043.946729618059</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44043.946926041666</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44043.947062581021</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44043.947199895832</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44043.947426550927</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>